<commit_message>
update with udbredelse af gødning
</commit_message>
<xml_diff>
--- a/output/udbred_poten_kt_Goedn_år.xlsx
+++ b/output/udbred_poten_kt_Goedn_år.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Scenarie</t>
   </si>
@@ -20,7 +20,10 @@
     <t xml:space="preserve">Dyr</t>
   </si>
   <si>
-    <t xml:space="preserve">TotGoednabDyr_kt_år</t>
+    <t xml:space="preserve">TotGoednabDyr_kt_år_pot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotGoedningabDyr_kt_år_udbr</t>
   </si>
   <si>
     <t xml:space="preserve">biogas</t>
@@ -407,258 +410,330 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
         <v>12567.5623329173</v>
       </c>
+      <c r="D2" t="n">
+        <v>3141.89058322933</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>10746.0999638823</v>
       </c>
+      <c r="D3" t="n">
+        <v>4827.9579547877</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>15709.4529161466</v>
       </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
         <v>15574.05791867</v>
       </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
         <v>15352.3363653232</v>
       </c>
+      <c r="D6" t="n">
+        <v>357.1165508235</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
         <v>6850.87325992317</v>
       </c>
+      <c r="D7" t="n">
+        <v>451.114122566825</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>14730.5081101332</v>
       </c>
+      <c r="D8" t="n">
+        <v>978.944806013418</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" t="n">
         <v>12253.3732745944</v>
       </c>
+      <c r="D9" t="n">
+        <v>3456.07964155226</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" t="n">
         <v>15709.4529161466</v>
       </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
         <v>15574.05791867</v>
       </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
         <v>10571.530990656</v>
       </c>
+      <c r="D12" t="n">
+        <v>1085.95563365066</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" t="n">
         <v>15709.4529161466</v>
       </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" t="n">
         <v>15574.05791867</v>
       </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" t="n">
         <v>13902.7031296754</v>
       </c>
+      <c r="D15" t="n">
+        <v>1085.95563365066</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" t="n">
         <v>7301.98738249</v>
       </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" t="n">
         <v>11122.1625037403</v>
       </c>
+      <c r="D17" t="n">
+        <v>3866.49625958574</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n">
         <v>5038.3712939181</v>
       </c>
+      <c r="D18" t="n">
+        <v>2263.6160885719</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" t="n">
         <v>13902.7031296754</v>
       </c>
+      <c r="D19" t="n">
+        <v>1085.95563365066</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" t="n">
         <v>7301.98738249</v>
       </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" t="n">
         <v>13902.7031296754</v>
       </c>
+      <c r="D21" t="n">
+        <v>1085.95563365066</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" t="n">
         <v>7301.98738249</v>
       </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
         <v>13902.7031296754</v>
       </c>
+      <c r="D23" t="n">
+        <v>1085.95563365066</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" t="n">
         <v>7301.98738249</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "update with udbredelse af gødning"
This reverts commit a834b43acb3f5f15389af38eb5cda27573885324.
</commit_message>
<xml_diff>
--- a/output/udbred_poten_kt_Goedn_år.xlsx
+++ b/output/udbred_poten_kt_Goedn_år.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Scenarie</t>
   </si>
@@ -20,10 +20,7 @@
     <t xml:space="preserve">Dyr</t>
   </si>
   <si>
-    <t xml:space="preserve">TotGoednabDyr_kt_år_pot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TotGoedningabDyr_kt_år_udbr</t>
+    <t xml:space="preserve">TotGoednabDyr_kt_år</t>
   </si>
   <si>
     <t xml:space="preserve">biogas</t>
@@ -410,330 +407,258 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
         <v>12567.5623329173</v>
       </c>
-      <c r="D2" t="n">
-        <v>3141.89058322933</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
         <v>10746.0999638823</v>
       </c>
-      <c r="D3" t="n">
-        <v>4827.9579547877</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="n">
         <v>15709.4529161466</v>
       </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" t="n">
         <v>15574.05791867</v>
       </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
         <v>15352.3363653232</v>
       </c>
-      <c r="D6" t="n">
-        <v>357.1165508235</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="n">
         <v>6850.87325992317</v>
       </c>
-      <c r="D7" t="n">
-        <v>451.114122566825</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
         <v>14730.5081101332</v>
       </c>
-      <c r="D8" t="n">
-        <v>978.944806013418</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="n">
         <v>12253.3732745944</v>
       </c>
-      <c r="D9" t="n">
-        <v>3456.07964155226</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="n">
         <v>15709.4529161466</v>
       </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
         <v>15574.05791867</v>
       </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" t="n">
         <v>10571.530990656</v>
       </c>
-      <c r="D12" t="n">
-        <v>1085.95563365066</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="n">
         <v>15709.4529161466</v>
       </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
         <v>15574.05791867</v>
       </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" t="n">
         <v>13902.7031296754</v>
       </c>
-      <c r="D15" t="n">
-        <v>1085.95563365066</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" t="n">
         <v>7301.98738249</v>
       </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" t="n">
         <v>11122.1625037403</v>
       </c>
-      <c r="D17" t="n">
-        <v>3866.49625958574</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
         <v>5038.3712939181</v>
       </c>
-      <c r="D18" t="n">
-        <v>2263.6160885719</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" t="n">
         <v>13902.7031296754</v>
       </c>
-      <c r="D19" t="n">
-        <v>1085.95563365066</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" t="n">
         <v>7301.98738249</v>
       </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" t="n">
         <v>13902.7031296754</v>
       </c>
-      <c r="D21" t="n">
-        <v>1085.95563365066</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="n">
         <v>7301.98738249</v>
       </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" t="n">
         <v>13902.7031296754</v>
       </c>
-      <c r="D23" t="n">
-        <v>1085.95563365066</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" t="n">
         <v>7301.98738249</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reapply "update with udbredelse af gødning"
This reverts commit db977c4d33547d1f3f8eb798e39a2a1e9e7ac616.
</commit_message>
<xml_diff>
--- a/output/udbred_poten_kt_Goedn_år.xlsx
+++ b/output/udbred_poten_kt_Goedn_år.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Scenarie</t>
   </si>
@@ -20,7 +20,10 @@
     <t xml:space="preserve">Dyr</t>
   </si>
   <si>
-    <t xml:space="preserve">TotGoednabDyr_kt_år</t>
+    <t xml:space="preserve">TotGoednabDyr_kt_år_pot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TotGoedningabDyr_kt_år_udbr</t>
   </si>
   <si>
     <t xml:space="preserve">biogas</t>
@@ -407,258 +410,330 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
         <v>12567.5623329173</v>
       </c>
+      <c r="D2" t="n">
+        <v>3141.89058322933</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>10746.0999638823</v>
       </c>
+      <c r="D3" t="n">
+        <v>4827.9579547877</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
         <v>15709.4529161466</v>
       </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
         <v>15574.05791867</v>
       </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
         <v>15352.3363653232</v>
       </c>
+      <c r="D6" t="n">
+        <v>357.1165508235</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
         <v>6850.87325992317</v>
       </c>
+      <c r="D7" t="n">
+        <v>451.114122566825</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>14730.5081101332</v>
       </c>
+      <c r="D8" t="n">
+        <v>978.944806013418</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" t="n">
         <v>12253.3732745944</v>
       </c>
+      <c r="D9" t="n">
+        <v>3456.07964155226</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" t="n">
         <v>15709.4529161466</v>
       </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
         <v>15574.05791867</v>
       </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
         <v>10571.530990656</v>
       </c>
+      <c r="D12" t="n">
+        <v>1085.95563365066</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" t="n">
         <v>15709.4529161466</v>
       </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" t="n">
         <v>15574.05791867</v>
       </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" t="n">
         <v>13902.7031296754</v>
       </c>
+      <c r="D15" t="n">
+        <v>1085.95563365066</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" t="n">
         <v>7301.98738249</v>
       </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C17" t="n">
         <v>11122.1625037403</v>
       </c>
+      <c r="D17" t="n">
+        <v>3866.49625958574</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n">
         <v>5038.3712939181</v>
       </c>
+      <c r="D18" t="n">
+        <v>2263.6160885719</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" t="n">
         <v>13902.7031296754</v>
       </c>
+      <c r="D19" t="n">
+        <v>1085.95563365066</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" t="n">
         <v>7301.98738249</v>
       </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" t="n">
         <v>13902.7031296754</v>
       </c>
+      <c r="D21" t="n">
+        <v>1085.95563365066</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" t="n">
         <v>7301.98738249</v>
       </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" t="n">
         <v>13902.7031296754</v>
       </c>
+      <c r="D23" t="n">
+        <v>1085.95563365066</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" t="n">
         <v>7301.98738249</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>